<commit_message>
Fixing issue #2: Normalize initial velocity of the bullet
</commit_message>
<xml_diff>
--- a/Exercises/Chapter 1/Results/Projectile-trajectory.xlsx
+++ b/Exercises/Chapter 1/Results/Projectile-trajectory.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simone/Documents/Projects/ray-tracer-challenge-netcore/Exercises/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ray-tracer-challenge-netcore\Exercises\Chapter 1\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1240" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="2205" yWindow="1245" windowWidth="28800" windowHeight="17595" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -69,12 +69,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -183,67 +186,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.99</c:v>
+                  <c:v>0.70710678118654702</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.97</c:v>
+                  <c:v>1.4042135623730001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.94</c:v>
+                  <c:v>2.0913203435596399</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9</c:v>
+                  <c:v>2.7684271247461898</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.85</c:v>
+                  <c:v>3.4355339059327399</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.79</c:v>
+                  <c:v>4.0926406871192897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.72</c:v>
+                  <c:v>4.73974746830583</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.64</c:v>
+                  <c:v>5.3768542494923803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.55</c:v>
+                  <c:v>6.0039610306789299</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.45</c:v>
+                  <c:v>6.6210678118654798</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.34</c:v>
+                  <c:v>7.22817459305202</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.22</c:v>
+                  <c:v>7.8252813742385703</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.09</c:v>
+                  <c:v>8.4123881554251199</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13.95</c:v>
+                  <c:v>8.9894949366116705</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14.8</c:v>
+                  <c:v>9.5566017177982108</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15.64</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>16.47</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>17.29</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>18.1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>18.9</c:v>
+                  <c:v>10.113708498984799</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -255,72 +246,65 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9</c:v>
+                  <c:v>1.7071067811865499</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7</c:v>
+                  <c:v>2.3142135623730899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4</c:v>
+                  <c:v>2.8213203435596399</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>3.2284271247461902</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.5</c:v>
+                  <c:v>3.53553390593274</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9</c:v>
+                  <c:v>3.7426406871192799</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.2</c:v>
+                  <c:v>3.8497474683058299</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.4</c:v>
+                  <c:v>3.8568542494923799</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.5</c:v>
+                  <c:v>3.7639610306789302</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5</c:v>
+                  <c:v>3.5710678118654799</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.4</c:v>
+                  <c:v>3.2781745930520199</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.2</c:v>
+                  <c:v>2.8852813742385699</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.9</c:v>
+                  <c:v>2.3923881554251198</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.5</c:v>
+                  <c:v>1.7994949366116699</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.0</c:v>
+                  <c:v>1.1066017177982099</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.7</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.9</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0</c:v>
+                  <c:v>0.31370849898476</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A499-49C4-A5A7-494C78B6C355}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -340,6 +324,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -401,6 +386,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1334,180 +1320,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1.99</v>
+        <v>0.70710678118654702</v>
       </c>
       <c r="B2">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1.7071067811865499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2.97</v>
+        <v>1.4042135623730001</v>
       </c>
       <c r="B3">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2.3142135623730899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3.94</v>
+        <v>2.0913203435596399</v>
       </c>
       <c r="B4">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2.8213203435596399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4.9000000000000004</v>
+        <v>2.7684271247461898</v>
       </c>
       <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3.2284271247461902</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5.85</v>
+        <v>3.4355339059327399</v>
       </c>
       <c r="B6">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3.53553390593274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6.79</v>
+        <v>4.0926406871192897</v>
       </c>
       <c r="B7">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3.7426406871192799</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7.72</v>
+        <v>4.73974746830583</v>
       </c>
       <c r="B8">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3.8497474683058299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8.64</v>
+        <v>5.3768542494923803</v>
       </c>
       <c r="B9">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3.8568542494923799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9.5500000000000007</v>
+        <v>6.0039610306789299</v>
       </c>
       <c r="B10">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3.7639610306789302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10.45</v>
+        <v>6.6210678118654798</v>
       </c>
       <c r="B11">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3.5710678118654799</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11.34</v>
+        <v>7.22817459305202</v>
       </c>
       <c r="B12">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3.2781745930520199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12.22</v>
+        <v>7.8252813742385703</v>
       </c>
       <c r="B13">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2.8852813742385699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13.09</v>
+        <v>8.4123881554251199</v>
       </c>
       <c r="B14">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2.3923881554251198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13.95</v>
+        <v>8.9894949366116705</v>
       </c>
       <c r="B15">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1.7994949366116699</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14.8</v>
+        <v>9.5566017177982108</v>
       </c>
       <c r="B16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1.1066017177982099</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15.64</v>
+        <v>10.113708498984799</v>
       </c>
       <c r="B17">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>16.47</v>
-      </c>
-      <c r="B18">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>17.29</v>
-      </c>
-      <c r="B19">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
+        <v>0.31370849898476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>